<commit_message>
added first set of draugr cards
</commit_message>
<xml_diff>
--- a/Doc/Units & Decks.xlsx
+++ b/Doc/Units & Decks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Unity Projects\SkyrimGwent2020 Repo\Skyrim_Gwent-V1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36299F84-5E7B-4039-AFFF-37D8DBCBF9FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1482C5-A816-44D6-A8F2-4F8429FF81AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B61D6D22-1838-4EC5-B1B5-63556785679F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="86">
   <si>
     <t>Deck: Whiterun</t>
   </si>
@@ -223,6 +223,72 @@
   </si>
   <si>
     <t>Guard Mage x2</t>
+  </si>
+  <si>
+    <t>Rag Draugr</t>
+  </si>
+  <si>
+    <t>Draugr</t>
+  </si>
+  <si>
+    <t>Draugr Archer</t>
+  </si>
+  <si>
+    <t>Restless Draugr</t>
+  </si>
+  <si>
+    <t>Deathlord</t>
+  </si>
+  <si>
+    <t>Scourgelord</t>
+  </si>
+  <si>
+    <t>Skeletal Dragon</t>
+  </si>
+  <si>
+    <t>frost mage</t>
+  </si>
+  <si>
+    <t>undead</t>
+  </si>
+  <si>
+    <t>Draugr Mob</t>
+  </si>
+  <si>
+    <t>Fierce Draugr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scourge </t>
+  </si>
+  <si>
+    <t>Dragon Priest</t>
+  </si>
+  <si>
+    <t>Ancient Nordic Draugr</t>
+  </si>
+  <si>
+    <t>Skeletal Archer</t>
+  </si>
+  <si>
+    <t>Draugr Overlord</t>
+  </si>
+  <si>
+    <t>Draugr wight</t>
+  </si>
+  <si>
+    <t>spellsword</t>
+  </si>
+  <si>
+    <t>Draugr Skirmisher</t>
+  </si>
+  <si>
+    <t>Wightlord</t>
+  </si>
+  <si>
+    <t>Red Eagle</t>
+  </si>
+  <si>
+    <t>gauldruson brother? One of them is an archer</t>
   </si>
 </sst>
 </file>
@@ -575,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646D0C0E-A598-41B5-948D-309EB21C6A27}">
-  <dimension ref="A3:H83"/>
+  <dimension ref="A3:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,66 +1410,434 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" t="s">
+        <v>32</v>
+      </c>
+      <c r="G63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" t="s">
+        <v>32</v>
+      </c>
+      <c r="G64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" t="s">
+        <v>32</v>
+      </c>
+      <c r="G65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>4</v>
+      </c>
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" t="s">
+        <v>32</v>
+      </c>
+      <c r="F66" t="s">
+        <v>32</v>
+      </c>
+      <c r="G66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="B67" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>19</v>
+      </c>
+      <c r="E67" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>6</v>
+      </c>
+      <c r="B68" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" t="s">
+        <v>32</v>
+      </c>
+      <c r="G68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>7</v>
+      </c>
+      <c r="B69" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69" t="s">
+        <v>19</v>
+      </c>
+      <c r="E69" t="s">
+        <v>32</v>
+      </c>
+      <c r="G69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>8</v>
+      </c>
+      <c r="B70" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" t="s">
+        <v>32</v>
+      </c>
+      <c r="G70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>9</v>
+      </c>
+      <c r="B71" t="s">
+        <v>83</v>
+      </c>
+      <c r="C71">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" t="s">
+        <v>32</v>
+      </c>
+      <c r="G71" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72">
+        <v>5</v>
+      </c>
+      <c r="D72" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" t="s">
+        <v>32</v>
+      </c>
+      <c r="G72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>11</v>
+      </c>
+      <c r="B73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" t="s">
+        <v>32</v>
+      </c>
+      <c r="G73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>12</v>
+      </c>
+      <c r="B74" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>2</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>1</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>6</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D77" t="s">
         <v>7</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E77" t="s">
         <v>12</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F77" t="s">
         <v>8</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G77" t="s">
         <v>21</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H77" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>5</v>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>76</v>
+      </c>
+      <c r="C78">
+        <v>13</v>
+      </c>
+      <c r="D78" t="s">
+        <v>71</v>
+      </c>
+      <c r="E78" t="s">
+        <v>32</v>
+      </c>
+      <c r="F78" t="s">
+        <v>32</v>
+      </c>
+      <c r="G78" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79" t="s">
+        <v>70</v>
+      </c>
+      <c r="C79">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>71</v>
+      </c>
+      <c r="E79" t="s">
+        <v>32</v>
+      </c>
+      <c r="F79" t="s">
+        <v>32</v>
+      </c>
+      <c r="G79" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>3</v>
+      </c>
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>71</v>
+      </c>
+      <c r="E80" t="s">
+        <v>32</v>
+      </c>
+      <c r="G80" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>4</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" t="s">
+        <v>32</v>
+      </c>
+      <c r="G81" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>2</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B84" t="s">
         <v>1</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C84" t="s">
         <v>6</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D84" t="s">
         <v>7</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
         <v>12</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F84" t="s">
         <v>8</v>
       </c>
-      <c r="G83" t="s">
+      <c r="G84" t="s">
         <v>21</v>
       </c>
-      <c r="H83" t="s">
+      <c r="H84" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85" t="s">
+        <v>66</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>30</v>
+      </c>
+      <c r="E85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>2</v>
+      </c>
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>30</v>
+      </c>
+      <c r="E86" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>3</v>
+      </c>
+      <c r="B87" t="s">
+        <v>78</v>
+      </c>
+      <c r="C87">
+        <v>1</v>
+      </c>
+      <c r="D87" t="s">
+        <v>30</v>
+      </c>
+      <c r="E87" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added first set of collegeOfWinterhold cards
</commit_message>
<xml_diff>
--- a/Doc/Units & Decks.xlsx
+++ b/Doc/Units & Decks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Unity Projects\SkyrimGwent2020 Repo\Skyrim_Gwent-V1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D22CF6-9A91-4DAF-A3BC-22CCDE445AB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB48DE6-6BC6-4C57-A67E-EE323C74432C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B61D6D22-1838-4EC5-B1B5-63556785679F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="117">
   <si>
     <t>Deck: Whiterun</t>
   </si>
@@ -294,9 +294,6 @@
     <t>Deck: College Of Winterhold</t>
   </si>
   <si>
-    <t>Consists of most mage cards. Pack a handfull of clear weathers &amp; frostbites</t>
-  </si>
-  <si>
     <t>Summons</t>
   </si>
   <si>
@@ -312,9 +309,6 @@
     <t>Potent Storm Atronach</t>
   </si>
   <si>
-    <t>Artifacts: Staff Of Magnus</t>
-  </si>
-  <si>
     <t>Packs a lot of warrior cards, and all weather cards</t>
   </si>
   <si>
@@ -325,6 +319,69 @@
   </si>
   <si>
     <t>Potent Frost Atronach</t>
+  </si>
+  <si>
+    <t>Artifacts: Staff Of Magnus, Sigil Stone (Summon a Powerful Daedra)</t>
+  </si>
+  <si>
+    <t>no images for mirabelle, collete, onmund</t>
+  </si>
+  <si>
+    <t>Brelyna Maryon</t>
+  </si>
+  <si>
+    <t>J'Zargo</t>
+  </si>
+  <si>
+    <t>fire mage</t>
+  </si>
+  <si>
+    <t>Phinis Gestor</t>
+  </si>
+  <si>
+    <t>Faralda</t>
+  </si>
+  <si>
+    <t>Drevis</t>
+  </si>
+  <si>
+    <t>Savos Aren</t>
+  </si>
+  <si>
+    <t>master conjurer</t>
+  </si>
+  <si>
+    <t>master destruction</t>
+  </si>
+  <si>
+    <t>master illusionist</t>
+  </si>
+  <si>
+    <t>master alteration</t>
+  </si>
+  <si>
+    <t>Consists of most mage cards. Pack a handfull of clear weathers &amp; frostbites, has more spellswords than warriors</t>
+  </si>
+  <si>
+    <t>Tolfdir (Spellsword)</t>
+  </si>
+  <si>
+    <t>Scorch but most likely might kill herself?</t>
+  </si>
+  <si>
+    <t>breton</t>
+  </si>
+  <si>
+    <t>summon a high level daedric warrior</t>
+  </si>
+  <si>
+    <t>altmer</t>
+  </si>
+  <si>
+    <t>dunmer</t>
+  </si>
+  <si>
+    <t>Spy card. (Do whenm spy cards are implemented)</t>
   </si>
 </sst>
 </file>
@@ -677,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646D0C0E-A598-41B5-948D-309EB21C6A27}">
-  <dimension ref="A1:H136"/>
+  <dimension ref="A1:H140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="H122" sqref="H122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,12 +754,12 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1901,12 +1958,12 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
@@ -1945,7 +2002,7 @@
         <v>1</v>
       </c>
       <c r="B98" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C98">
         <v>4</v>
@@ -1957,7 +2014,7 @@
         <v>32</v>
       </c>
       <c r="G98" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.3">
@@ -1965,7 +2022,7 @@
         <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C99">
         <v>6</v>
@@ -1977,54 +2034,64 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100">
-        <v>3</v>
-      </c>
-    </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B101" t="s">
+        <v>110</v>
+      </c>
+      <c r="C101">
+        <v>8</v>
+      </c>
+      <c r="D101" t="s">
+        <v>108</v>
+      </c>
+      <c r="E101" t="s">
+        <v>32</v>
+      </c>
+      <c r="G101" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A109">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.3">
@@ -2063,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="B113" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -2075,7 +2142,7 @@
         <v>32</v>
       </c>
       <c r="G113" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.3">
@@ -2083,7 +2150,7 @@
         <v>2</v>
       </c>
       <c r="B114" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C114">
         <v>4</v>
@@ -2095,7 +2162,7 @@
         <v>32</v>
       </c>
       <c r="G114" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.3">
@@ -2103,7 +2170,7 @@
         <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C115">
         <v>5</v>
@@ -2115,7 +2182,7 @@
         <v>32</v>
       </c>
       <c r="G115" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.3">
@@ -2123,7 +2190,7 @@
         <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C116">
         <v>7</v>
@@ -2135,47 +2202,114 @@
         <v>32</v>
       </c>
       <c r="G116" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <v>5</v>
+        <v>87</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>98</v>
+      </c>
+      <c r="C118">
+        <v>4</v>
+      </c>
+      <c r="D118" t="s">
+        <v>100</v>
+      </c>
+      <c r="E118" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B119" t="s">
+        <v>99</v>
+      </c>
+      <c r="C119">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s">
+        <v>100</v>
+      </c>
+      <c r="E119" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A120">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B120" t="s">
+        <v>101</v>
+      </c>
+      <c r="C120">
+        <v>9</v>
+      </c>
+      <c r="D120" t="s">
+        <v>105</v>
+      </c>
+      <c r="E120" t="s">
+        <v>32</v>
+      </c>
+      <c r="G120" t="s">
+        <v>112</v>
+      </c>
+      <c r="H120" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A121">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B121" t="s">
+        <v>102</v>
+      </c>
+      <c r="C121">
+        <v>8</v>
+      </c>
+      <c r="D121" t="s">
+        <v>106</v>
+      </c>
+      <c r="E121" t="s">
+        <v>32</v>
+      </c>
+      <c r="G121" t="s">
+        <v>114</v>
+      </c>
+      <c r="H121" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A122">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A123">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A124">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B124" t="s">
+        <v>104</v>
+      </c>
+      <c r="C124">
+        <v>11</v>
+      </c>
+      <c r="D124" t="s">
+        <v>71</v>
+      </c>
+      <c r="F124" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.3">
@@ -2209,44 +2343,70 @@
         <v>9</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
+        <v>103</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129" t="s">
+        <v>107</v>
+      </c>
+      <c r="E129" t="s">
+        <v>32</v>
+      </c>
+      <c r="F129" t="s">
+        <v>32</v>
+      </c>
+      <c r="G129" t="s">
+        <v>115</v>
+      </c>
+      <c r="H129" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>4</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>8</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added melee units for Wilderness Deck
</commit_message>
<xml_diff>
--- a/Doc/Units & Decks.xlsx
+++ b/Doc/Units & Decks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Unity Projects\SkyrimGwent2020 Repo\Skyrim_Gwent-V1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB48DE6-6BC6-4C57-A67E-EE323C74432C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EB5052-D2DC-4670-9EE5-52E8DC2976F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B61D6D22-1838-4EC5-B1B5-63556785679F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="147">
   <si>
     <t>Deck: Whiterun</t>
   </si>
@@ -382,6 +382,96 @@
   </si>
   <si>
     <t>Spy card. (Do whenm spy cards are implemented)</t>
+  </si>
+  <si>
+    <t>##########################################################################################################</t>
+  </si>
+  <si>
+    <t>Deck: Wilderness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Artifacts: </t>
+  </si>
+  <si>
+    <t>Creatures</t>
+  </si>
+  <si>
+    <t>Ash Spawn</t>
+  </si>
+  <si>
+    <t>charus</t>
+  </si>
+  <si>
+    <t>archer</t>
+  </si>
+  <si>
+    <t>creatures</t>
+  </si>
+  <si>
+    <t>troll</t>
+  </si>
+  <si>
+    <t>frost troll</t>
+  </si>
+  <si>
+    <t>ice wraith</t>
+  </si>
+  <si>
+    <t>ice mage</t>
+  </si>
+  <si>
+    <t>wolf</t>
+  </si>
+  <si>
+    <t>ice wolf</t>
+  </si>
+  <si>
+    <t>mammoth</t>
+  </si>
+  <si>
+    <t>sabrecat</t>
+  </si>
+  <si>
+    <t>skeever</t>
+  </si>
+  <si>
+    <t>spriggan</t>
+  </si>
+  <si>
+    <t>spriggan matron</t>
+  </si>
+  <si>
+    <t>spriggan earth mother</t>
+  </si>
+  <si>
+    <t>healer</t>
+  </si>
+  <si>
+    <t>wispmother</t>
+  </si>
+  <si>
+    <t>werewolf</t>
+  </si>
+  <si>
+    <t>falmer archer</t>
+  </si>
+  <si>
+    <t>hagraven</t>
+  </si>
+  <si>
+    <t>glenmorin witch</t>
+  </si>
+  <si>
+    <t>charus hunter</t>
+  </si>
+  <si>
+    <t>udefrykte(named troll)</t>
+  </si>
+  <si>
+    <t>fierce sabrecat</t>
+  </si>
+  <si>
+    <t>giant</t>
   </si>
 </sst>
 </file>
@@ -734,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646D0C0E-A598-41B5-948D-309EB21C6A27}">
-  <dimension ref="A1:H140"/>
+  <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="H122" sqref="H122"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="G157" sqref="G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2409,6 +2499,483 @@
         <v>97</v>
       </c>
     </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1</v>
+      </c>
+      <c r="C150" t="s">
+        <v>6</v>
+      </c>
+      <c r="D150" t="s">
+        <v>7</v>
+      </c>
+      <c r="E150" t="s">
+        <v>12</v>
+      </c>
+      <c r="F150" t="s">
+        <v>8</v>
+      </c>
+      <c r="G150" t="s">
+        <v>21</v>
+      </c>
+      <c r="H150" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151" t="s">
+        <v>121</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+      <c r="D151" t="s">
+        <v>20</v>
+      </c>
+      <c r="E151" t="s">
+        <v>32</v>
+      </c>
+      <c r="G151" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <v>2</v>
+      </c>
+      <c r="B152" t="s">
+        <v>125</v>
+      </c>
+      <c r="C152">
+        <v>3</v>
+      </c>
+      <c r="D152" t="s">
+        <v>20</v>
+      </c>
+      <c r="E152" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <v>3</v>
+      </c>
+      <c r="B153" t="s">
+        <v>126</v>
+      </c>
+      <c r="C153">
+        <v>4</v>
+      </c>
+      <c r="D153" t="s">
+        <v>19</v>
+      </c>
+      <c r="E153" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <v>4</v>
+      </c>
+      <c r="B154" t="s">
+        <v>144</v>
+      </c>
+      <c r="C154">
+        <v>5</v>
+      </c>
+      <c r="D154" t="s">
+        <v>19</v>
+      </c>
+      <c r="E154" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <v>5</v>
+      </c>
+      <c r="B155" t="s">
+        <v>129</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+      <c r="D155" t="s">
+        <v>20</v>
+      </c>
+      <c r="E155" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <v>6</v>
+      </c>
+      <c r="B156" t="s">
+        <v>131</v>
+      </c>
+      <c r="C156">
+        <v>5</v>
+      </c>
+      <c r="D156" t="s">
+        <v>19</v>
+      </c>
+      <c r="E156" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <v>7</v>
+      </c>
+      <c r="B157" t="s">
+        <v>132</v>
+      </c>
+      <c r="C157">
+        <v>6</v>
+      </c>
+      <c r="D157" t="s">
+        <v>19</v>
+      </c>
+      <c r="E157" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <v>8</v>
+      </c>
+      <c r="B158" t="s">
+        <v>133</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158" t="s">
+        <v>20</v>
+      </c>
+      <c r="E158" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A159">
+        <v>9</v>
+      </c>
+      <c r="B159" t="s">
+        <v>139</v>
+      </c>
+      <c r="C159">
+        <v>8</v>
+      </c>
+      <c r="D159" t="s">
+        <v>19</v>
+      </c>
+      <c r="E159" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A160">
+        <v>10</v>
+      </c>
+      <c r="B160" t="s">
+        <v>130</v>
+      </c>
+      <c r="C160">
+        <v>3</v>
+      </c>
+      <c r="D160" t="s">
+        <v>20</v>
+      </c>
+      <c r="E160" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A161">
+        <v>11</v>
+      </c>
+      <c r="B161" t="s">
+        <v>145</v>
+      </c>
+      <c r="C161">
+        <v>7</v>
+      </c>
+      <c r="D161" t="s">
+        <v>19</v>
+      </c>
+      <c r="E161" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A162">
+        <v>12</v>
+      </c>
+      <c r="B162" t="s">
+        <v>146</v>
+      </c>
+      <c r="C162">
+        <v>9</v>
+      </c>
+      <c r="D162" t="s">
+        <v>19</v>
+      </c>
+      <c r="E162" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A165" t="s">
+        <v>2</v>
+      </c>
+      <c r="B165" t="s">
+        <v>1</v>
+      </c>
+      <c r="C165" t="s">
+        <v>6</v>
+      </c>
+      <c r="D165" t="s">
+        <v>7</v>
+      </c>
+      <c r="E165" t="s">
+        <v>12</v>
+      </c>
+      <c r="F165" t="s">
+        <v>8</v>
+      </c>
+      <c r="G165" t="s">
+        <v>21</v>
+      </c>
+      <c r="H165" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A166">
+        <v>1</v>
+      </c>
+      <c r="B166" t="s">
+        <v>127</v>
+      </c>
+      <c r="C166">
+        <v>6</v>
+      </c>
+      <c r="D166" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A167">
+        <v>2</v>
+      </c>
+      <c r="B167" t="s">
+        <v>134</v>
+      </c>
+      <c r="C167">
+        <v>4</v>
+      </c>
+      <c r="D167" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A168">
+        <v>3</v>
+      </c>
+      <c r="B168" t="s">
+        <v>135</v>
+      </c>
+      <c r="C168">
+        <v>7</v>
+      </c>
+      <c r="D168" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A169">
+        <v>4</v>
+      </c>
+      <c r="B169" t="s">
+        <v>136</v>
+      </c>
+      <c r="C169">
+        <v>10</v>
+      </c>
+      <c r="D169" t="s">
+        <v>137</v>
+      </c>
+      <c r="F169" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A170">
+        <v>5</v>
+      </c>
+      <c r="B170" t="s">
+        <v>138</v>
+      </c>
+      <c r="C170">
+        <v>11</v>
+      </c>
+      <c r="D170" t="s">
+        <v>52</v>
+      </c>
+      <c r="F170" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A171">
+        <v>6</v>
+      </c>
+      <c r="B171" t="s">
+        <v>141</v>
+      </c>
+      <c r="C171">
+        <v>5</v>
+      </c>
+      <c r="D171" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A172">
+        <v>7</v>
+      </c>
+      <c r="B172" t="s">
+        <v>142</v>
+      </c>
+      <c r="C172">
+        <v>8</v>
+      </c>
+      <c r="D172" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
+        <v>2</v>
+      </c>
+      <c r="B181" t="s">
+        <v>1</v>
+      </c>
+      <c r="C181" t="s">
+        <v>6</v>
+      </c>
+      <c r="D181" t="s">
+        <v>7</v>
+      </c>
+      <c r="E181" t="s">
+        <v>12</v>
+      </c>
+      <c r="F181" t="s">
+        <v>8</v>
+      </c>
+      <c r="G181" t="s">
+        <v>21</v>
+      </c>
+      <c r="H181" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>1</v>
+      </c>
+      <c r="B182" t="s">
+        <v>122</v>
+      </c>
+      <c r="C182">
+        <v>3</v>
+      </c>
+      <c r="D182" t="s">
+        <v>123</v>
+      </c>
+      <c r="G182" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>4</v>
+      </c>
+      <c r="B185" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
created deck prefab for wilderness deck
</commit_message>
<xml_diff>
--- a/Doc/Units & Decks.xlsx
+++ b/Doc/Units & Decks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Unity Projects\SkyrimGwent2020 Repo\Skyrim_Gwent-V1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EB5052-D2DC-4670-9EE5-52E8DC2976F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1531EAD1-D2B5-4478-9FF9-D24DD58E8B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B61D6D22-1838-4EC5-B1B5-63556785679F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="147">
   <si>
     <t>Deck: Whiterun</t>
   </si>
@@ -827,7 +827,7 @@
   <dimension ref="A1:H189"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="G157" sqref="G157"/>
+      <selection activeCell="E172" sqref="E172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2791,11 +2791,14 @@
         <v>127</v>
       </c>
       <c r="C166">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D166" t="s">
         <v>128</v>
       </c>
+      <c r="E166" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167">
@@ -2809,6 +2812,9 @@
       </c>
       <c r="D167" t="s">
         <v>137</v>
+      </c>
+      <c r="E167" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
@@ -2824,6 +2830,9 @@
       <c r="D168" t="s">
         <v>137</v>
       </c>
+      <c r="E168" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169">
@@ -2838,6 +2847,9 @@
       <c r="D169" t="s">
         <v>137</v>
       </c>
+      <c r="E169" t="s">
+        <v>32</v>
+      </c>
       <c r="F169" t="s">
         <v>32</v>
       </c>
@@ -2855,6 +2867,9 @@
       <c r="D170" t="s">
         <v>52</v>
       </c>
+      <c r="E170" t="s">
+        <v>32</v>
+      </c>
       <c r="F170" t="s">
         <v>32</v>
       </c>
@@ -2872,6 +2887,9 @@
       <c r="D171" t="s">
         <v>100</v>
       </c>
+      <c r="E171" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A172">
@@ -2885,6 +2903,9 @@
       </c>
       <c r="D172" t="s">
         <v>100</v>
+      </c>
+      <c r="E172" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
made wilderness deck a bit stronger
</commit_message>
<xml_diff>
--- a/Doc/Units & Decks.xlsx
+++ b/Doc/Units & Decks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Unity Projects\SkyrimGwent2020 Repo\Skyrim_Gwent-V1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1531EAD1-D2B5-4478-9FF9-D24DD58E8B29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE9541-BCC0-4464-9573-295B77974D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B61D6D22-1838-4EC5-B1B5-63556785679F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="149">
   <si>
     <t>Deck: Whiterun</t>
   </si>
@@ -399,9 +399,6 @@
     <t>Ash Spawn</t>
   </si>
   <si>
-    <t>charus</t>
-  </si>
-  <si>
     <t>archer</t>
   </si>
   <si>
@@ -472,6 +469,15 @@
   </si>
   <si>
     <t>giant</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>charus reaper</t>
+  </si>
+  <si>
+    <t>on discard or scorch, summons a hunter if not alread deployed</t>
   </si>
 </sst>
 </file>
@@ -826,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646D0C0E-A598-41B5-948D-309EB21C6A27}">
   <dimension ref="A1:H189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="E172" sqref="E172"/>
+    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="H182" sqref="H182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2570,7 +2576,7 @@
         <v>2</v>
       </c>
       <c r="B152" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C152">
         <v>3</v>
@@ -2587,7 +2593,7 @@
         <v>3</v>
       </c>
       <c r="B153" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C153">
         <v>4</v>
@@ -2604,7 +2610,7 @@
         <v>4</v>
       </c>
       <c r="B154" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C154">
         <v>5</v>
@@ -2621,7 +2627,7 @@
         <v>5</v>
       </c>
       <c r="B155" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C155">
         <v>2</v>
@@ -2638,7 +2644,7 @@
         <v>6</v>
       </c>
       <c r="B156" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C156">
         <v>5</v>
@@ -2655,7 +2661,7 @@
         <v>7</v>
       </c>
       <c r="B157" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C157">
         <v>6</v>
@@ -2672,7 +2678,7 @@
         <v>8</v>
       </c>
       <c r="B158" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C158">
         <v>1</v>
@@ -2689,7 +2695,7 @@
         <v>9</v>
       </c>
       <c r="B159" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C159">
         <v>8</v>
@@ -2706,7 +2712,7 @@
         <v>10</v>
       </c>
       <c r="B160" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C160">
         <v>3</v>
@@ -2723,7 +2729,7 @@
         <v>11</v>
       </c>
       <c r="B161" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C161">
         <v>7</v>
@@ -2740,7 +2746,7 @@
         <v>12</v>
       </c>
       <c r="B162" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C162">
         <v>9</v>
@@ -2788,13 +2794,13 @@
         <v>1</v>
       </c>
       <c r="B166" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C166">
         <v>3</v>
       </c>
       <c r="D166" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E166" t="s">
         <v>32</v>
@@ -2805,13 +2811,13 @@
         <v>2</v>
       </c>
       <c r="B167" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C167">
         <v>4</v>
       </c>
       <c r="D167" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E167" t="s">
         <v>32</v>
@@ -2822,13 +2828,13 @@
         <v>3</v>
       </c>
       <c r="B168" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C168">
         <v>7</v>
       </c>
       <c r="D168" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E168" t="s">
         <v>32</v>
@@ -2839,13 +2845,13 @@
         <v>4</v>
       </c>
       <c r="B169" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C169">
         <v>10</v>
       </c>
       <c r="D169" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E169" t="s">
         <v>32</v>
@@ -2859,7 +2865,7 @@
         <v>5</v>
       </c>
       <c r="B170" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C170">
         <v>11</v>
@@ -2879,7 +2885,7 @@
         <v>6</v>
       </c>
       <c r="B171" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C171">
         <v>5</v>
@@ -2888,7 +2894,7 @@
         <v>100</v>
       </c>
       <c r="E171" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
@@ -2896,7 +2902,7 @@
         <v>7</v>
       </c>
       <c r="B172" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C172">
         <v>8</v>
@@ -2905,7 +2911,7 @@
         <v>100</v>
       </c>
       <c r="E172" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
@@ -2944,16 +2950,22 @@
         <v>1</v>
       </c>
       <c r="B182" t="s">
+        <v>147</v>
+      </c>
+      <c r="C182">
+        <v>5</v>
+      </c>
+      <c r="D182" t="s">
         <v>122</v>
       </c>
-      <c r="C182">
-        <v>3</v>
-      </c>
-      <c r="D182" t="s">
+      <c r="E182" t="s">
+        <v>32</v>
+      </c>
+      <c r="G182" t="s">
         <v>123</v>
       </c>
-      <c r="G182" t="s">
-        <v>124</v>
+      <c r="H182" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
@@ -2966,7 +2978,10 @@
         <v>3</v>
       </c>
       <c r="B184" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="E184" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
@@ -2974,7 +2989,16 @@
         <v>4</v>
       </c>
       <c r="B185" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="C185">
+        <v>3</v>
+      </c>
+      <c r="D185" t="s">
+        <v>122</v>
+      </c>
+      <c r="E185" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added first set of thalmor cards
</commit_message>
<xml_diff>
--- a/Doc/Units & Decks.xlsx
+++ b/Doc/Units & Decks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Unity Projects\SkyrimGwent2020 Repo\Skyrim_Gwent-V1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE9541-BCC0-4464-9573-295B77974D5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43C547D-4E8D-4DE7-9C13-C00D61C0389D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B61D6D22-1838-4EC5-B1B5-63556785679F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="172">
   <si>
     <t>Deck: Whiterun</t>
   </si>
@@ -478,6 +478,75 @@
   </si>
   <si>
     <t>on discard or scorch, summons a hunter if not alread deployed</t>
+  </si>
+  <si>
+    <t>Deck: Thalmor</t>
+  </si>
+  <si>
+    <t>Thalmor Wizard</t>
+  </si>
+  <si>
+    <t>Thalmor Archer</t>
+  </si>
+  <si>
+    <t>Thalmor Soldier</t>
+  </si>
+  <si>
+    <t>Northwatch Archer</t>
+  </si>
+  <si>
+    <t>Northwatch Mage</t>
+  </si>
+  <si>
+    <t>Northwatch Guard</t>
+  </si>
+  <si>
+    <t>Northwatch Interogater</t>
+  </si>
+  <si>
+    <t>Shavari</t>
+  </si>
+  <si>
+    <t>Spy</t>
+  </si>
+  <si>
+    <t>Khajiit</t>
+  </si>
+  <si>
+    <t>Ancano</t>
+  </si>
+  <si>
+    <t>Thalmor Agent</t>
+  </si>
+  <si>
+    <t>Elenwen a leader card</t>
+  </si>
+  <si>
+    <t>Estormo</t>
+  </si>
+  <si>
+    <t>Lorcalin</t>
+  </si>
+  <si>
+    <t>Ondolemar</t>
+  </si>
+  <si>
+    <t>Justicar</t>
+  </si>
+  <si>
+    <t>bound blade assassin</t>
+  </si>
+  <si>
+    <t>warrior</t>
+  </si>
+  <si>
+    <t>spellsword 1</t>
+  </si>
+  <si>
+    <t>spellsword 2</t>
+  </si>
+  <si>
+    <t>rulindil</t>
   </si>
 </sst>
 </file>
@@ -830,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646D0C0E-A598-41B5-948D-309EB21C6A27}">
-  <dimension ref="A1:H189"/>
+  <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="H182" sqref="H182"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="F212" sqref="F212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3021,6 +3090,428 @@
         <v>8</v>
       </c>
     </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B196" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B198" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>2</v>
+      </c>
+      <c r="B201" t="s">
+        <v>1</v>
+      </c>
+      <c r="C201" t="s">
+        <v>6</v>
+      </c>
+      <c r="D201" t="s">
+        <v>7</v>
+      </c>
+      <c r="E201" t="s">
+        <v>12</v>
+      </c>
+      <c r="F201" t="s">
+        <v>8</v>
+      </c>
+      <c r="G201" t="s">
+        <v>21</v>
+      </c>
+      <c r="H201" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>1</v>
+      </c>
+      <c r="B202" t="s">
+        <v>152</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="E202" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>2</v>
+      </c>
+      <c r="B203" t="s">
+        <v>155</v>
+      </c>
+      <c r="C203">
+        <v>2</v>
+      </c>
+      <c r="E203" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>3</v>
+      </c>
+      <c r="B204" t="s">
+        <v>161</v>
+      </c>
+      <c r="C204">
+        <v>3</v>
+      </c>
+      <c r="E204" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>4</v>
+      </c>
+      <c r="B205" t="s">
+        <v>165</v>
+      </c>
+      <c r="C205">
+        <v>4</v>
+      </c>
+      <c r="D205" t="s">
+        <v>158</v>
+      </c>
+      <c r="E205" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>5</v>
+      </c>
+      <c r="B206" t="s">
+        <v>166</v>
+      </c>
+      <c r="C206">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>6</v>
+      </c>
+      <c r="B207" t="s">
+        <v>167</v>
+      </c>
+      <c r="C207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>7</v>
+      </c>
+      <c r="B208" t="s">
+        <v>168</v>
+      </c>
+      <c r="C208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>8</v>
+      </c>
+      <c r="B209" t="s">
+        <v>171</v>
+      </c>
+      <c r="C209">
+        <v>7</v>
+      </c>
+      <c r="E209" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>2</v>
+      </c>
+      <c r="B216" t="s">
+        <v>1</v>
+      </c>
+      <c r="C216" t="s">
+        <v>6</v>
+      </c>
+      <c r="D216" t="s">
+        <v>7</v>
+      </c>
+      <c r="E216" t="s">
+        <v>12</v>
+      </c>
+      <c r="F216" t="s">
+        <v>8</v>
+      </c>
+      <c r="G216" t="s">
+        <v>21</v>
+      </c>
+      <c r="H216" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>1</v>
+      </c>
+      <c r="B217" t="s">
+        <v>150</v>
+      </c>
+      <c r="C217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>2</v>
+      </c>
+      <c r="B218" t="s">
+        <v>154</v>
+      </c>
+      <c r="C218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>3</v>
+      </c>
+      <c r="B219" t="s">
+        <v>156</v>
+      </c>
+      <c r="C219">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>4</v>
+      </c>
+      <c r="B220" t="s">
+        <v>160</v>
+      </c>
+      <c r="C220">
+        <v>0</v>
+      </c>
+      <c r="D220" t="s">
+        <v>158</v>
+      </c>
+      <c r="E220" t="s">
+        <v>32</v>
+      </c>
+      <c r="F220" t="s">
+        <v>32</v>
+      </c>
+      <c r="G220" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>5</v>
+      </c>
+      <c r="B221" t="s">
+        <v>163</v>
+      </c>
+      <c r="C221">
+        <v>6</v>
+      </c>
+      <c r="D221" t="s">
+        <v>158</v>
+      </c>
+      <c r="E221" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>7</v>
+      </c>
+      <c r="B223" t="s">
+        <v>169</v>
+      </c>
+      <c r="C223">
+        <v>4</v>
+      </c>
+      <c r="E223" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>8</v>
+      </c>
+      <c r="B224" t="s">
+        <v>170</v>
+      </c>
+      <c r="C224">
+        <v>6</v>
+      </c>
+      <c r="E224" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>2</v>
+      </c>
+      <c r="B232" t="s">
+        <v>1</v>
+      </c>
+      <c r="C232" t="s">
+        <v>6</v>
+      </c>
+      <c r="D232" t="s">
+        <v>7</v>
+      </c>
+      <c r="E232" t="s">
+        <v>12</v>
+      </c>
+      <c r="F232" t="s">
+        <v>8</v>
+      </c>
+      <c r="G232" t="s">
+        <v>21</v>
+      </c>
+      <c r="H232" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>1</v>
+      </c>
+      <c r="B233" t="s">
+        <v>151</v>
+      </c>
+      <c r="C233">
+        <v>2</v>
+      </c>
+      <c r="E233" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>2</v>
+      </c>
+      <c r="B234" t="s">
+        <v>153</v>
+      </c>
+      <c r="C234">
+        <v>3</v>
+      </c>
+      <c r="E234" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>3</v>
+      </c>
+      <c r="B235" t="s">
+        <v>157</v>
+      </c>
+      <c r="C235">
+        <v>6</v>
+      </c>
+      <c r="D235" t="s">
+        <v>158</v>
+      </c>
+      <c r="E235" t="s">
+        <v>32</v>
+      </c>
+      <c r="G235" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>4</v>
+      </c>
+      <c r="B236" t="s">
+        <v>164</v>
+      </c>
+      <c r="C236">
+        <v>8</v>
+      </c>
+      <c r="D236" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added theif card images
</commit_message>
<xml_diff>
--- a/Doc/Units & Decks.xlsx
+++ b/Doc/Units & Decks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Unity Projects\SkyrimGwent2020 Repo\Skyrim_Gwent-V1\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43C547D-4E8D-4DE7-9C13-C00D61C0389D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A236FE7-D775-4D0D-8635-62E9F6B5D30A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B61D6D22-1838-4EC5-B1B5-63556785679F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="204">
   <si>
     <t>Deck: Whiterun</t>
   </si>
@@ -547,6 +547,102 @@
   </si>
   <si>
     <t>rulindil</t>
+  </si>
+  <si>
+    <t>Deck: Thieves Guild</t>
+  </si>
+  <si>
+    <t>Maven Black Briar Leader card</t>
+  </si>
+  <si>
+    <t>red guard looter x2</t>
+  </si>
+  <si>
+    <t>corrupt guard skirmisher x2</t>
+  </si>
+  <si>
+    <t>corrupt guard x2</t>
+  </si>
+  <si>
+    <t>guild archer</t>
+  </si>
+  <si>
+    <t>thief</t>
+  </si>
+  <si>
+    <t>khajjit thief</t>
+  </si>
+  <si>
+    <t>fence</t>
+  </si>
+  <si>
+    <t>argonian thief</t>
+  </si>
+  <si>
+    <t>argonian archer</t>
+  </si>
+  <si>
+    <t>argonian picklocker</t>
+  </si>
+  <si>
+    <t>dirge</t>
+  </si>
+  <si>
+    <t>maul</t>
+  </si>
+  <si>
+    <t>hireling</t>
+  </si>
+  <si>
+    <t>Mauricio (hireling)</t>
+  </si>
+  <si>
+    <t>Karliah</t>
+  </si>
+  <si>
+    <t>Mercer Frey</t>
+  </si>
+  <si>
+    <t>Turn into nightingale</t>
+  </si>
+  <si>
+    <t>brynjolf</t>
+  </si>
+  <si>
+    <t>No Images:</t>
+  </si>
+  <si>
+    <t>Vipir The Fleet</t>
+  </si>
+  <si>
+    <t>gallus desidenius</t>
+  </si>
+  <si>
+    <t>spy</t>
+  </si>
+  <si>
+    <t>gulum Ei</t>
+  </si>
+  <si>
+    <t>gian the fist</t>
+  </si>
+  <si>
+    <t>vex</t>
+  </si>
+  <si>
+    <t>tonilia</t>
+  </si>
+  <si>
+    <t>delvin</t>
+  </si>
+  <si>
+    <t>no images</t>
+  </si>
+  <si>
+    <t>thrynn, rune</t>
+  </si>
+  <si>
+    <t>cynric endell</t>
   </si>
 </sst>
 </file>
@@ -899,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646D0C0E-A598-41B5-948D-309EB21C6A27}">
-  <dimension ref="A1:H240"/>
+  <dimension ref="A1:H298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
-      <selection activeCell="F212" sqref="F212"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="C258" sqref="C258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3512,6 +3608,380 @@
         <v>8</v>
       </c>
     </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B246" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B248" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>2</v>
+      </c>
+      <c r="B251" t="s">
+        <v>1</v>
+      </c>
+      <c r="C251" t="s">
+        <v>6</v>
+      </c>
+      <c r="D251" t="s">
+        <v>7</v>
+      </c>
+      <c r="E251" t="s">
+        <v>12</v>
+      </c>
+      <c r="F251" t="s">
+        <v>8</v>
+      </c>
+      <c r="G251" t="s">
+        <v>21</v>
+      </c>
+      <c r="H251" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>1</v>
+      </c>
+      <c r="B252" t="s">
+        <v>176</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>2</v>
+      </c>
+      <c r="B253" t="s">
+        <v>175</v>
+      </c>
+      <c r="C253">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>3</v>
+      </c>
+      <c r="B254" t="s">
+        <v>174</v>
+      </c>
+      <c r="C254">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>4</v>
+      </c>
+      <c r="B255" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>5</v>
+      </c>
+      <c r="B256" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>6</v>
+      </c>
+      <c r="B257" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>7</v>
+      </c>
+      <c r="B258" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>8</v>
+      </c>
+      <c r="B259" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>9</v>
+      </c>
+      <c r="B260" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B262" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B263" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>2</v>
+      </c>
+      <c r="B266" t="s">
+        <v>1</v>
+      </c>
+      <c r="C266" t="s">
+        <v>6</v>
+      </c>
+      <c r="D266" t="s">
+        <v>7</v>
+      </c>
+      <c r="E266" t="s">
+        <v>12</v>
+      </c>
+      <c r="F266" t="s">
+        <v>8</v>
+      </c>
+      <c r="G266" t="s">
+        <v>21</v>
+      </c>
+      <c r="H266" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>1</v>
+      </c>
+      <c r="B267" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>2</v>
+      </c>
+      <c r="B268" t="s">
+        <v>187</v>
+      </c>
+      <c r="C268">
+        <v>5</v>
+      </c>
+      <c r="D268" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>2</v>
+      </c>
+      <c r="B282" t="s">
+        <v>1</v>
+      </c>
+      <c r="C282" t="s">
+        <v>6</v>
+      </c>
+      <c r="D282" t="s">
+        <v>7</v>
+      </c>
+      <c r="E282" t="s">
+        <v>12</v>
+      </c>
+      <c r="F282" t="s">
+        <v>8</v>
+      </c>
+      <c r="G282" t="s">
+        <v>21</v>
+      </c>
+      <c r="H282" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>1</v>
+      </c>
+      <c r="B283" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>2</v>
+      </c>
+      <c r="B284" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>3</v>
+      </c>
+      <c r="B285" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>4</v>
+      </c>
+      <c r="B286" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>5</v>
+      </c>
+      <c r="B287" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>6</v>
+      </c>
+      <c r="B288" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>7</v>
+      </c>
+      <c r="B289" t="s">
+        <v>188</v>
+      </c>
+      <c r="H289" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>8</v>
+      </c>
+      <c r="B290" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>9</v>
+      </c>
+      <c r="B291" t="s">
+        <v>196</v>
+      </c>
+      <c r="C291">
+        <v>2</v>
+      </c>
+      <c r="D291" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B293" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>9</v>
+      </c>
+      <c r="B294" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>10</v>
+      </c>
+      <c r="B295" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>11</v>
+      </c>
+      <c r="B296" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>12</v>
+      </c>
+      <c r="B297" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B298" t="s">
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>